<commit_message>
Adding velocity as a 2nd objective
</commit_message>
<xml_diff>
--- a/Dissertation Experiments.xlsx
+++ b/Dissertation Experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Pranav/Desktop/dissertation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A6BF99-8258-854B-A125-38BC5183B6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB7A532-6D08-194E-BA38-63487243E475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{91207AF7-D7AD-544E-8EFB-458CF7CA4CC0}"/>
   </bookViews>
@@ -491,7 +491,7 @@
   <dimension ref="A2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>